<commit_message>
Supplemented the SUMMON LOG FORMAT section of README.md
</commit_message>
<xml_diff>
--- a/genshin.xlsx
+++ b/genshin.xlsx
@@ -1159,7 +1159,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -1239,7 +1239,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -1266,7 +1266,7 @@
             </a:defRPr>
           </a:pPr>
           <a:r>
-            <a:t/>
+            <a:t>None</a:t>
           </a:r>
           <a:endParaRPr lang="en-US"/>
         </a:p>
@@ -1796,7 +1796,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -1876,7 +1876,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -1903,7 +1903,7 @@
             </a:defRPr>
           </a:pPr>
           <a:r>
-            <a:t/>
+            <a:t>None</a:t>
           </a:r>
           <a:endParaRPr lang="en-US"/>
         </a:p>
@@ -1960,7 +1960,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:t/>
+                  <a:t>None</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
@@ -2051,7 +2051,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:t/>
+                  <a:t>None</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
@@ -2142,7 +2142,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:t/>
+                  <a:t>None</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
@@ -2256,7 +2256,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -2340,7 +2340,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -2366,7 +2366,7 @@
             </a:defRPr>
           </a:pPr>
           <a:r>
-            <a:t/>
+            <a:t>None</a:t>
           </a:r>
           <a:endParaRPr lang="en-US"/>
         </a:p>

</xml_diff>